<commit_message>
Tests - attributeValueCss - MainPageTest_VerifyMainMenu
</commit_message>
<xml_diff>
--- a/Test Cases - Excel Files/Scenariusz Testowy - Weryfikacja menu głównego.xlsx
+++ b/Test Cases - Excel Files/Scenariusz Testowy - Weryfikacja menu głównego.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD6F5DB-257C-4D35-BBB4-94387547734C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97341F9-DD60-40C7-A23E-12EB39CE3127}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
   <si>
     <t>Nazwa Scenariusza Testowego</t>
   </si>
@@ -23,9 +23,6 @@
     <t>Osoba przeprowadzająca test</t>
   </si>
   <si>
-    <t>Data</t>
-  </si>
-  <si>
     <t>Nr</t>
   </si>
   <si>
@@ -56,73 +53,40 @@
     <t>Przedmiot testów</t>
   </si>
   <si>
-    <t>Wejdź na główną stronę sklepu.</t>
-  </si>
-  <si>
-    <t>Strona główna sklepu wyświetlona</t>
-  </si>
-  <si>
     <t>OK</t>
   </si>
   <si>
     <t>2.</t>
   </si>
   <si>
-    <t>Zweryfikuj tytuł strony.</t>
-  </si>
-  <si>
     <t>1.</t>
   </si>
   <si>
     <t>3.</t>
   </si>
   <si>
-    <t>Zweryfikuj czy menu główne składa się z prawidłowej ilości zakładek.</t>
-  </si>
-  <si>
-    <t>Poprawna ilość zakładek w menu to 4.</t>
-  </si>
-  <si>
     <t>Menu składa się z 4 zakładek</t>
   </si>
   <si>
     <t>4.</t>
   </si>
   <si>
-    <t>Zweryfikuj czy menu główne zawiera następujące zakładki: Aktualności, Opinie o sklepie, Reklamacje, Kontakt.</t>
-  </si>
-  <si>
     <t>Menu główne zawiera następujące zakładki: Aktualności, Opinie o sklepie, Reklamacje, Kontakt.</t>
   </si>
   <si>
     <t>5.</t>
   </si>
   <si>
-    <t>Zweryfikuj czy zakładki w menu głównym są wyświetlane w prawidłowej kolejności.</t>
-  </si>
-  <si>
     <t>Poprawna kolejnośc zakładek w menu głównym (patrząć od lewej do prawej): Aktualności, Opinie o sklepie, Reklamacje, Kontakt</t>
   </si>
   <si>
     <t>Kolejnośc zakładek w menu głównym (patrząć od lewej do prawej): Aktualności, Opinie o sklepie, Reklamacje, Kontakt</t>
   </si>
   <si>
-    <t>6.</t>
-  </si>
-  <si>
     <t>Sprawdz czy każdna z zakładek w menu głownym, po kliknięciu przekierowuje na odpowiednie podstrony(adresy www)</t>
   </si>
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>Adres głównej strony sklepu: http://koszulkifootball.sellingo.pl/</t>
-  </si>
-  <si>
-    <t>Poprawny tytuł strony to: 'Koszulkifootball.sellingo.pl'</t>
-  </si>
-  <si>
-    <t>Tytuł strony: ''Koszulkifootball.sellingo.pl''</t>
   </si>
   <si>
     <t>Każda z zakładek przekierowuje na odpowienia podstronę (adres www):
@@ -140,6 +104,64 @@
   </si>
   <si>
     <t>Sklep internetowy http://koszulkifootball.sellingo.pl/</t>
+  </si>
+  <si>
+    <t>Autor Scenariusza Testowego</t>
+  </si>
+  <si>
+    <t>Wejdź na główną stronę sklepu i zweryfikuj tytuł strony</t>
+  </si>
+  <si>
+    <t>Adres głównej strony sklepu: http://koszulkifootball.sellingo.pl/
+Poprawny tytuł strony to: 'Koszulkifootball.sellingo.pl'</t>
+  </si>
+  <si>
+    <t>Strona główna sklepu wyświetlona
+Tytuł strony: ''Koszulkifootball.sellingo.pl''</t>
+  </si>
+  <si>
+    <t>Poprawna ilość zakładek w menu to 4</t>
+  </si>
+  <si>
+    <t>Zweryfikuj czy menu główne składa się z prawidłowej ilości zakładek</t>
+  </si>
+  <si>
+    <t>Zweryfikuj czy menu główne zawiera następujące zakładki: Aktualności, Opinie o sklepie, Reklamacje, Kontakt</t>
+  </si>
+  <si>
+    <t>Zweryfikuj czy zakładki w menu głównym są wyświetlane w prawidłowej kolejności</t>
+  </si>
+  <si>
+    <t>6.</t>
+  </si>
+  <si>
+    <t>Zakładki mają właściwości:
+kolor tekstu: rgba(255, 255, 255, 1)
+kolor tła: rgba(55, 55, 55, 1)</t>
+  </si>
+  <si>
+    <t>7.</t>
+  </si>
+  <si>
+    <t>Zweryfikuj czy każda z zakładek w menu ma prawidłowe własciwości (kolor tekstu i kolor tła)</t>
+  </si>
+  <si>
+    <t>Zweryfikuj czy każda z zakładek w menu, po najechaniu na nią myszką, zmienia kolor tekstu oraz tła na prawidowy.</t>
+  </si>
+  <si>
+    <t>Prawidłowe właściwości(kolor tekstu i kolor tła) zakładek w menu, po najechaniu myszką to:
+kolor tekstu: rgba(255, 255, 255, 1)
+kolor tła: rgba(55, 55, 55, 1)</t>
+  </si>
+  <si>
+    <t>Prawidłowe właściwości(kolor tekstu i kolor tła) zakładek w menu to:
+kolor tekstu: rgba(55, 55, 55, 1)
+kolor tła: rgbargba(0, 0, 0, 0)</t>
+  </si>
+  <si>
+    <t>Zakładki mają właściwości:
+kolor tekstu: rgba(55, 55, 55, 1)
+kolor tła: rgbargba(0, 0, 0, 0)</t>
   </si>
 </sst>
 </file>
@@ -199,7 +221,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -283,10 +305,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -301,7 +323,22 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -313,36 +350,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -388,85 +395,102 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -474,13 +498,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -489,32 +510,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -854,10 +863,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:H12"/>
+  <dimension ref="B1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,226 +882,245 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="17"/>
+      <c r="B2" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="15"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="23"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="18"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="23"/>
-    </row>
-    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="24">
-        <v>43401</v>
-      </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="26"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="18"/>
     </row>
     <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="D6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="E6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="F6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="G6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="H6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="15" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="7" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>15</v>
+        <v>30</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="F8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+      <c r="F10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>32</v>
-      </c>
+      <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="22"/>
     </row>
-    <row r="12" spans="2:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="8" t="s">
+    <row r="12" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="22"/>
+    </row>
+    <row r="13" spans="2:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>32</v>
+      <c r="C13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="D2:H2"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D3:H3"/>
-    <mergeCell ref="D4:H4"/>
     <mergeCell ref="D5:H5"/>
     <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Refactor MainPage.class and MainPageTest (wait expected condition)
</commit_message>
<xml_diff>
--- a/Test Cases - Excel Files/Scenariusz Testowy - Weryfikacja menu głównego.xlsx
+++ b/Test Cases - Excel Files/Scenariusz Testowy - Weryfikacja menu głównego.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97341F9-DD60-40C7-A23E-12EB39CE3127}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27E3F11-3BB4-43F7-990B-CF7D75602750}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>OK</t>
   </si>
   <si>
-    <t>2.</t>
-  </si>
-  <si>
     <t>1.</t>
   </si>
   <si>
@@ -109,17 +106,10 @@
     <t>Autor Scenariusza Testowego</t>
   </si>
   <si>
-    <t>Wejdź na główną stronę sklepu i zweryfikuj tytuł strony</t>
-  </si>
-  <si>
     <t>Adres głównej strony sklepu: http://koszulkifootball.sellingo.pl/
 Poprawny tytuł strony to: 'Koszulkifootball.sellingo.pl'</t>
   </si>
   <si>
-    <t>Strona główna sklepu wyświetlona
-Tytuł strony: ''Koszulkifootball.sellingo.pl''</t>
-  </si>
-  <si>
     <t>Poprawna ilość zakładek w menu to 4</t>
   </si>
   <si>
@@ -135,18 +125,10 @@
     <t>6.</t>
   </si>
   <si>
-    <t>Zakładki mają właściwości:
-kolor tekstu: rgba(255, 255, 255, 1)
-kolor tła: rgba(55, 55, 55, 1)</t>
-  </si>
-  <si>
     <t>7.</t>
   </si>
   <si>
     <t>Zweryfikuj czy każda z zakładek w menu ma prawidłowe własciwości (kolor tekstu i kolor tła)</t>
-  </si>
-  <si>
-    <t>Zweryfikuj czy każda z zakładek w menu, po najechaniu na nią myszką, zmienia kolor tekstu oraz tła na prawidowy.</t>
   </si>
   <si>
     <t>Prawidłowe właściwości(kolor tekstu i kolor tła) zakładek w menu, po najechaniu myszką to:
@@ -162,6 +144,27 @@
     <t>Zakładki mają właściwości:
 kolor tekstu: rgba(55, 55, 55, 1)
 kolor tła: rgbargba(0, 0, 0, 0)</t>
+  </si>
+  <si>
+    <t>Strona główna sklepu wyświetlona
+Tytuł strony: ''Koszulkifootball.sellingo.pl''
+Pliki Cookies usunięte
+Zrzut ekranu zapisany do pliku .jpg</t>
+  </si>
+  <si>
+    <t>Wejdź na główną stronę sklepu, usuń pliki cookies i zweryfikuj tytuł strony. Dodatkowo wykonaj zrzut ekranu.</t>
+  </si>
+  <si>
+    <t>Zweryfikuj czy każda z zakładek w menu, po najechaniu na nią myszką, zmienia kolor tekstu oraz tła na prawidowy. Dodatkowo wykonaj zrzut ekranu</t>
+  </si>
+  <si>
+    <t>Zakładki mają właściwości:
+kolor tekstu: rgba(255, 255, 255, 1)
+kolor tła: rgba(55, 55, 55, 1)
+Zrzut ekranu zapisany do pliku .jpg</t>
+  </si>
+  <si>
+    <t>2.</t>
   </si>
 </sst>
 </file>
@@ -498,6 +501,15 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -515,15 +527,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -865,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,56 +885,56 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="15"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17" t="s">
+      <c r="C3" s="20"/>
+      <c r="D3" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="18"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="21"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17" t="s">
+      <c r="B4" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="18"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="21"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17" t="s">
+      <c r="C5" s="20"/>
+      <c r="D5" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="18"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="21"/>
     </row>
     <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="11" t="s">
@@ -958,157 +961,157 @@
     </row>
     <row r="7" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>12</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>12</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="F10" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>42</v>
+        <v>18</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>37</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="22"/>
+      <c r="H11" s="16"/>
     </row>
     <row r="12" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="21" t="s">
+      <c r="E12" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="22"/>
+      <c r="H12" s="16"/>
     </row>
     <row r="13" spans="2:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>12</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>